<commit_message>
I am finally sure that the traslocation is fine, and it is described in grid.py in lines 685-699
</commit_message>
<xml_diff>
--- a/SP_means.xlsx
+++ b/SP_means.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\luciana_datos\UCI\Project_14 (Anna)\DEMENT_gradcatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63B0067-2282-4371-AC7F-96E832EF0531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED98AFA3-9FBA-4A59-A723-289475A1128D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>